<commit_message>
Changes after the two reviews
</commit_message>
<xml_diff>
--- a/Lesson 1/Project1/stroopdata.xlsx
+++ b/Lesson 1/Project1/stroopdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Udacity Course\Data Analysis\Lesson 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Udacity Course\Data Analysis\Lesson 1\Project1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Congruent</t>
   </si>
@@ -71,6 +71,36 @@
   </si>
   <si>
     <t>Seconds</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Box 2 - lower</t>
+  </si>
+  <si>
+    <t>Box 1 - hidden</t>
+  </si>
+  <si>
+    <t>Box 3 - upper</t>
+  </si>
+  <si>
+    <t>Whisker top</t>
+  </si>
+  <si>
+    <t>Whisker bottom</t>
   </si>
 </sst>
 </file>
@@ -697,7 +727,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -846,11 +875,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="258919888"/>
-        <c:axId val="258917648"/>
+        <c:axId val="255403536"/>
+        <c:axId val="255404096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="258919888"/>
+        <c:axId val="255403536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -872,14 +901,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="258917648"/>
+        <c:crossAx val="255404096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -887,7 +915,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="258917648"/>
+        <c:axId val="255404096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,14 +937,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="258919888"/>
+        <c:crossAx val="255403536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -971,7 +998,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1150,11 +1176,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="59935520"/>
-        <c:axId val="59936080"/>
+        <c:axId val="254497824"/>
+        <c:axId val="254498384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59935520"/>
+        <c:axId val="254497824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,14 +1202,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59936080"/>
+        <c:crossAx val="254498384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1191,7 +1216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59936080"/>
+        <c:axId val="254498384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,21 +1238,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59935520"/>
+        <c:crossAx val="254497824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1299,7 +1322,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1478,11 +1500,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="340360320"/>
-        <c:axId val="340362000"/>
+        <c:axId val="254500624"/>
+        <c:axId val="254501184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="340360320"/>
+        <c:axId val="254500624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1504,14 +1526,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="340362000"/>
+        <c:crossAx val="254501184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1519,7 +1540,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="340362000"/>
+        <c:axId val="254501184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,14 +1562,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="340360320"/>
+        <c:crossAx val="254500624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1557,7 +1577,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1573,6 +1592,533 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-BR"/>
+              <a:t>Samples</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-BR" baseline="0"/>
+              <a:t> Box-Plot</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stroopdata!$L$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Box 1 - hidden</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>stroopdata!$M$16:$O$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.26525</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.0297499999999982</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.6955000000000009</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>stroopdata!$M$4:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Congruent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Incongruent</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stroopdata!$M$11:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>11.895250000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.716749999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6455000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stroopdata!$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Box 2 - lower</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>stroopdata!$M$4:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Congruent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Incongruent</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stroopdata!$M$12:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.4612499999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3007500000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.020999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>stroopdata!$L$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Box 3 - upper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="65000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>stroopdata!$M$15:$O$15</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.1272500000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>11.203500000000005</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>11.660499999999997</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>stroopdata!$M$4:$O$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Congruent</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Incongruent</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Difference</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>stroopdata!$M$13:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.8442499999999988</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0339999999999989</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5920000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="305374704"/>
+        <c:axId val="305375264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="305374704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="305375264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="305375264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="305374704"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -1629,7 +2175,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1808,11 +2353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="457987600"/>
-        <c:axId val="457988160"/>
+        <c:axId val="254503424"/>
+        <c:axId val="254503984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457987600"/>
+        <c:axId val="254503424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1834,14 +2379,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457988160"/>
+        <c:crossAx val="254503984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1849,7 +2393,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="457988160"/>
+        <c:axId val="254503984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1871,14 +2415,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457987600"/>
+        <c:crossAx val="254503424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -1897,7 +2440,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -1934,7 +2477,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2113,11 +2655,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="457987040"/>
-        <c:axId val="314058960"/>
+        <c:axId val="254506224"/>
+        <c:axId val="254506784"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457987040"/>
+        <c:axId val="254506224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2139,14 +2681,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="314058960"/>
+        <c:crossAx val="254506784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2154,7 +2695,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314058960"/>
+        <c:axId val="254506784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,14 +2717,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457987040"/>
+        <c:crossAx val="254506224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2200,7 +2740,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
@@ -2246,7 +2786,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2395,11 +2934,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="345103552"/>
-        <c:axId val="347210144"/>
+        <c:axId val="254509024"/>
+        <c:axId val="254509584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="345103552"/>
+        <c:axId val="254509024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2421,14 +2960,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="347210144"/>
+        <c:crossAx val="254509584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2436,7 +2974,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="347210144"/>
+        <c:axId val="254509584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2458,14 +2996,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="345103552"/>
+        <c:crossAx val="254509024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2481,6 +3018,551 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2589,6 +3671,41 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3537,10 +4654,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N502"/>
+  <dimension ref="A1:O502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P18" sqref="N15:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3549,9 +4666,13 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -3562,7 +4683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3578,7 +4699,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3594,7 +4715,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3612,8 +4733,17 @@
         <v>0</v>
       </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3635,8 +4765,23 @@
         <v>2</v>
       </c>
       <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <f>MIN(B2:B25)</f>
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N5:O5" si="1">MIN(C2:C25)</f>
+        <v>15.686999999999999</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>1.9499999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3654,12 +4799,27 @@
         <v>10</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I26" si="1">I5+2</f>
+        <f t="shared" ref="I6:I24" si="2">I5+2</f>
         <v>4</v>
       </c>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6">
+        <f>QUARTILE(B2:B25,1)</f>
+        <v>11.895250000000001</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:O6" si="3">QUARTILE(C2:C25,1)</f>
+        <v>18.716749999999998</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>3.6455000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3677,12 +4837,27 @@
         <v>15</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <f>MEDIAN(B2:B25)</f>
+        <v>14.3565</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ref="N7:O7" si="4">MEDIAN(C2:C25)</f>
+        <v>21.017499999999998</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="4"/>
+        <v>7.6664999999999992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3700,12 +4875,27 @@
         <v>20</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M8">
+        <f>QUARTILE(B2:B25,3)</f>
+        <v>16.200749999999999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ref="N8:O8" si="5">QUARTILE(C2:C25,3)</f>
+        <v>24.051499999999997</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="5"/>
+        <v>10.2585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3723,12 +4913,27 @@
         <v>25</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9">
+        <f>MAX(B2:B25)</f>
+        <v>22.327999999999999</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ref="N9:O9" si="6">MAX(C2:C25)</f>
+        <v>35.255000000000003</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="6"/>
+        <v>21.918999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3743,12 +4948,12 @@
         <v>11.361000000000001</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3763,12 +4968,27 @@
         <v>11.802</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <f>M6</f>
+        <v>11.895250000000001</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:O11" si="7">N6</f>
+        <v>18.716749999999998</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="7"/>
+        <v>3.6455000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3783,12 +5003,27 @@
         <v>2.1960000000000015</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <f>M7-M6</f>
+        <v>2.4612499999999997</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ref="N12:O12" si="8">N7-N6</f>
+        <v>2.3007500000000007</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="8"/>
+        <v>4.020999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3803,12 +5038,27 @@
         <v>3.3459999999999983</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13">
+        <f>M8-M7</f>
+        <v>1.8442499999999988</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ref="N13:O13" si="9">N8-N7</f>
+        <v>3.0339999999999989</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="9"/>
+        <v>2.5920000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3823,12 +5073,12 @@
         <v>2.4370000000000012</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3843,12 +5093,27 @@
         <v>3.4009999999999998</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15">
+        <f>M9-M8</f>
+        <v>6.1272500000000001</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ref="N15:O15" si="10">N9-N8</f>
+        <v>11.203500000000005</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="10"/>
+        <v>11.660499999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3863,10 +5128,25 @@
         <v>17.055000000000003</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="J16" s="1"/>
+      <c r="L16" t="s">
+        <v>24</v>
+      </c>
+      <c r="M16">
+        <f>M6-M5</f>
+        <v>3.26525</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ref="N16:O16" si="11">N6-N5</f>
+        <v>3.0297499999999982</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="11"/>
+        <v>1.6955000000000009</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
@@ -3883,7 +5163,7 @@
         <v>10.028</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="J17" s="1"/>
@@ -3903,7 +5183,7 @@
         <v>6.6439999999999984</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="J18" s="1"/>
@@ -3923,7 +5203,7 @@
         <v>9.7899999999999991</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="J19" s="1"/>
@@ -3943,7 +5223,7 @@
         <v>6.0810000000000013</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="J20" s="1"/>
@@ -3963,7 +5243,7 @@
         <v>21.918999999999997</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="J21" s="1"/>
@@ -3983,7 +5263,7 @@
         <v>10.949999999999998</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="J22" s="1"/>
@@ -4009,7 +5289,7 @@
         <v>3.7270000000000003</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38</v>
       </c>
       <c r="J23" s="1"/>
@@ -4038,7 +5318,7 @@
         <v>12</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="J24" s="1"/>
@@ -4091,11 +5371,11 @@
         <v>14.051125000000001</v>
       </c>
       <c r="C26">
-        <f t="shared" ref="C26:D26" si="2">AVERAGE(C2:C25)</f>
+        <f t="shared" ref="C26:D26" si="12">AVERAGE(C2:C25)</f>
         <v>22.015916666666669</v>
       </c>
       <c r="D26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="12"/>
         <v>7.964791666666664</v>
       </c>
       <c r="F26">
@@ -4120,11 +5400,11 @@
         <v>14.3565</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:D27" si="3">MEDIAN(C2:C25)</f>
+        <f t="shared" ref="C27:D27" si="13">MEDIAN(C2:C25)</f>
         <v>21.017499999999998</v>
       </c>
       <c r="D27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>7.6664999999999992</v>
       </c>
       <c r="J27" s="1"/>
@@ -4145,11 +5425,11 @@
         <v>3.559357957645187</v>
       </c>
       <c r="C28">
-        <f t="shared" ref="C28:D28" si="4">_xlfn.STDEV.S(C2:C25)</f>
+        <f t="shared" ref="C28:D28" si="14">_xlfn.STDEV.S(C2:C25)</f>
         <v>4.7970571224691367</v>
       </c>
       <c r="D28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="14"/>
         <v>4.8648269103590565</v>
       </c>
       <c r="J28" s="1"/>
@@ -4163,11 +5443,11 @@
         <v>12.669029070652117</v>
       </c>
       <c r="C29">
-        <f t="shared" ref="C29:D29" si="5">C28^2</f>
+        <f t="shared" ref="C29:D29" si="15">C28^2</f>
         <v>23.011757036231874</v>
       </c>
       <c r="D29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="15"/>
         <v>23.666540867753643</v>
       </c>
       <c r="J29" s="1"/>
@@ -5601,16 +6881,17 @@
       </c>
       <c r="M502">
         <f>SUM(M2:M501)</f>
-        <v>0</v>
+        <v>99.003749999999997</v>
       </c>
       <c r="N502">
         <f>M502</f>
-        <v>0</v>
+        <v>99.003749999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>